<commit_message>
[Feat] 모든 작물 Asset Multiple하기
</commit_message>
<xml_diff>
--- a/Assets/02.Scripts/02.Item/Datas/ItemDatas.xlsx
+++ b/Assets/02.Scripts/02.Item/Datas/ItemDatas.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\unity\Become_Celebrity_on_Farm\Assets\02.Scripts\02.Item\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866AFEA9-42C2-4345-B6F6-C698BDF8FB02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFA2987C-A91C-448B-8320-D74006398655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11145" yWindow="1335" windowWidth="16320" windowHeight="13755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ItemDatas" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="303">
   <si>
     <t>이름</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -782,6 +782,397 @@
   </si>
   <si>
     <t>TreeSeed</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>딸기</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>딸기 씨</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>대파</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>대파 씨</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>감자</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>감자 씨</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>양파</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>양파 씨</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>당근</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>당근 씨</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>블루베리</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>블루베리 씨</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>무</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>무 씨</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>양배추</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>양배추 씨</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>콜리플라워</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>콜리플라워 씨</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>밀</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>밀 씨</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>브로콜리</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>브로콜리 씨</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Strawberry</t>
+  </si>
+  <si>
+    <t>Strawberry_Seed</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Greenonion</t>
+  </si>
+  <si>
+    <t>Onion</t>
+  </si>
+  <si>
+    <t>Carrot</t>
+  </si>
+  <si>
+    <t>Blueberry</t>
+  </si>
+  <si>
+    <t>Radish</t>
+  </si>
+  <si>
+    <t>Cabbage</t>
+  </si>
+  <si>
+    <t>Cauliflower</t>
+  </si>
+  <si>
+    <t>Wheat</t>
+  </si>
+  <si>
+    <t>Broccoli</t>
+  </si>
+  <si>
+    <t>Potato</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Greenonion_Seed</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Potato_Seed</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Onion_Seed</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Carrot_Seed</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Blueberry_Seed</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Radish_Seed</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cabbage_Seed</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wheat_Seed</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cauliflower_Seed</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Broccoli_Seed</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>토마토</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>토마토 씨</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>해바라기</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>해바라기 씨</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>고추</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>고추 씨</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>옥수수</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>옥수수 씨</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>노란 파프리카</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>노란 파프리카 씨</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>초록 파프리카</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>초록 파프리카 씨</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>빨간 파프리카</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>빨간 파프리카 씨</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>용과</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>용과 씨</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>수박</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>수박 씨</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>오이</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>오이 씨</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>가지</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>가지 씨</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>파인애플</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>파인애플 씨</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>완두콩</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>완두콩 씨</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>파란 작물</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>파란 작물 씨</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>쌀</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>쌀 씨</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tomato</t>
+  </si>
+  <si>
+    <t>Sunflower</t>
+  </si>
+  <si>
+    <t>Pepper</t>
+  </si>
+  <si>
+    <t>Corn</t>
+  </si>
+  <si>
+    <t>YelloPaprika</t>
+  </si>
+  <si>
+    <t>GreenPaprika</t>
+  </si>
+  <si>
+    <t>RedPaprika</t>
+  </si>
+  <si>
+    <t>Dragonfruit</t>
+  </si>
+  <si>
+    <t>Watermelon</t>
+  </si>
+  <si>
+    <t>Cucumber</t>
+  </si>
+  <si>
+    <t>Eggplant</t>
+  </si>
+  <si>
+    <t>Pineapple</t>
+  </si>
+  <si>
+    <t>Pea</t>
+  </si>
+  <si>
+    <t>Bluecrops</t>
+  </si>
+  <si>
+    <t>Rice</t>
+  </si>
+  <si>
+    <t>Tomato_Seed</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sunflower_Seed</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pepper_Seed</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Corn_Seed</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>YelloPaprika_Seed</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>GreenPaprika_Seed</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RedPaprika_Seed</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dragonfruit_Seed</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Watermelon_Seed</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cucumber_Seed</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Eggplant_Seed</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pineapple_Seed</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pea_Seed</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bluecrops_Seed</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rice_Seed</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1734,10 +2125,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L74"/>
+  <dimension ref="A1:L126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F75" sqref="F75"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3462,6 +3853,1202 @@
         <v>196</v>
       </c>
     </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>199</v>
+      </c>
+      <c r="C75" t="s">
+        <v>199</v>
+      </c>
+      <c r="D75" t="s">
+        <v>11</v>
+      </c>
+      <c r="E75">
+        <v>1</v>
+      </c>
+      <c r="F75">
+        <v>64</v>
+      </c>
+      <c r="L75" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>200</v>
+      </c>
+      <c r="C76" t="s">
+        <v>200</v>
+      </c>
+      <c r="D76" t="s">
+        <v>158</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="F76">
+        <v>64</v>
+      </c>
+      <c r="L76" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>201</v>
+      </c>
+      <c r="C77" t="s">
+        <v>201</v>
+      </c>
+      <c r="D77" t="s">
+        <v>11</v>
+      </c>
+      <c r="E77">
+        <v>1</v>
+      </c>
+      <c r="F77">
+        <v>64</v>
+      </c>
+      <c r="L77" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>202</v>
+      </c>
+      <c r="C78" t="s">
+        <v>202</v>
+      </c>
+      <c r="D78" t="s">
+        <v>158</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
+      <c r="F78">
+        <v>64</v>
+      </c>
+      <c r="L78" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>203</v>
+      </c>
+      <c r="C79" t="s">
+        <v>203</v>
+      </c>
+      <c r="D79" t="s">
+        <v>11</v>
+      </c>
+      <c r="E79">
+        <v>1</v>
+      </c>
+      <c r="F79">
+        <v>64</v>
+      </c>
+      <c r="L79" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>204</v>
+      </c>
+      <c r="C80" t="s">
+        <v>204</v>
+      </c>
+      <c r="D80" t="s">
+        <v>158</v>
+      </c>
+      <c r="E80">
+        <v>1</v>
+      </c>
+      <c r="F80">
+        <v>64</v>
+      </c>
+      <c r="L80" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>205</v>
+      </c>
+      <c r="C81" t="s">
+        <v>205</v>
+      </c>
+      <c r="D81" t="s">
+        <v>11</v>
+      </c>
+      <c r="E81">
+        <v>1</v>
+      </c>
+      <c r="F81">
+        <v>64</v>
+      </c>
+      <c r="L81" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>206</v>
+      </c>
+      <c r="C82" t="s">
+        <v>206</v>
+      </c>
+      <c r="D82" t="s">
+        <v>158</v>
+      </c>
+      <c r="E82">
+        <v>1</v>
+      </c>
+      <c r="F82">
+        <v>64</v>
+      </c>
+      <c r="L82" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>207</v>
+      </c>
+      <c r="C83" t="s">
+        <v>207</v>
+      </c>
+      <c r="D83" t="s">
+        <v>11</v>
+      </c>
+      <c r="E83">
+        <v>1</v>
+      </c>
+      <c r="F83">
+        <v>64</v>
+      </c>
+      <c r="L83" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>208</v>
+      </c>
+      <c r="C84" t="s">
+        <v>208</v>
+      </c>
+      <c r="D84" t="s">
+        <v>158</v>
+      </c>
+      <c r="E84">
+        <v>1</v>
+      </c>
+      <c r="F84">
+        <v>64</v>
+      </c>
+      <c r="L84" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>209</v>
+      </c>
+      <c r="C85" t="s">
+        <v>209</v>
+      </c>
+      <c r="D85" t="s">
+        <v>11</v>
+      </c>
+      <c r="E85">
+        <v>1</v>
+      </c>
+      <c r="F85">
+        <v>64</v>
+      </c>
+      <c r="L85" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>210</v>
+      </c>
+      <c r="C86" t="s">
+        <v>210</v>
+      </c>
+      <c r="D86" t="s">
+        <v>158</v>
+      </c>
+      <c r="E86">
+        <v>1</v>
+      </c>
+      <c r="F86">
+        <v>64</v>
+      </c>
+      <c r="L86" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>211</v>
+      </c>
+      <c r="C87" t="s">
+        <v>211</v>
+      </c>
+      <c r="D87" t="s">
+        <v>11</v>
+      </c>
+      <c r="E87">
+        <v>1</v>
+      </c>
+      <c r="F87">
+        <v>64</v>
+      </c>
+      <c r="L87" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>212</v>
+      </c>
+      <c r="C88" t="s">
+        <v>212</v>
+      </c>
+      <c r="D88" t="s">
+        <v>158</v>
+      </c>
+      <c r="E88">
+        <v>1</v>
+      </c>
+      <c r="F88">
+        <v>64</v>
+      </c>
+      <c r="L88" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>213</v>
+      </c>
+      <c r="C89" t="s">
+        <v>213</v>
+      </c>
+      <c r="D89" t="s">
+        <v>11</v>
+      </c>
+      <c r="E89">
+        <v>1</v>
+      </c>
+      <c r="F89">
+        <v>64</v>
+      </c>
+      <c r="L89" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>214</v>
+      </c>
+      <c r="C90" t="s">
+        <v>214</v>
+      </c>
+      <c r="D90" t="s">
+        <v>158</v>
+      </c>
+      <c r="E90">
+        <v>1</v>
+      </c>
+      <c r="F90">
+        <v>64</v>
+      </c>
+      <c r="L90" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>215</v>
+      </c>
+      <c r="C91" t="s">
+        <v>215</v>
+      </c>
+      <c r="D91" t="s">
+        <v>11</v>
+      </c>
+      <c r="E91">
+        <v>1</v>
+      </c>
+      <c r="F91">
+        <v>64</v>
+      </c>
+      <c r="L91" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>216</v>
+      </c>
+      <c r="C92" t="s">
+        <v>216</v>
+      </c>
+      <c r="D92" t="s">
+        <v>158</v>
+      </c>
+      <c r="E92">
+        <v>1</v>
+      </c>
+      <c r="F92">
+        <v>64</v>
+      </c>
+      <c r="L92" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>217</v>
+      </c>
+      <c r="C93" t="s">
+        <v>217</v>
+      </c>
+      <c r="D93" t="s">
+        <v>11</v>
+      </c>
+      <c r="E93">
+        <v>1</v>
+      </c>
+      <c r="F93">
+        <v>64</v>
+      </c>
+      <c r="L93" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>218</v>
+      </c>
+      <c r="C94" t="s">
+        <v>218</v>
+      </c>
+      <c r="D94" t="s">
+        <v>158</v>
+      </c>
+      <c r="E94">
+        <v>1</v>
+      </c>
+      <c r="F94">
+        <v>64</v>
+      </c>
+      <c r="L94" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>219</v>
+      </c>
+      <c r="C95" t="s">
+        <v>219</v>
+      </c>
+      <c r="D95" t="s">
+        <v>11</v>
+      </c>
+      <c r="E95">
+        <v>1</v>
+      </c>
+      <c r="F95">
+        <v>64</v>
+      </c>
+      <c r="L95" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>220</v>
+      </c>
+      <c r="C96" t="s">
+        <v>220</v>
+      </c>
+      <c r="D96" t="s">
+        <v>158</v>
+      </c>
+      <c r="E96">
+        <v>1</v>
+      </c>
+      <c r="F96">
+        <v>64</v>
+      </c>
+      <c r="L96" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>243</v>
+      </c>
+      <c r="C97" t="s">
+        <v>243</v>
+      </c>
+      <c r="D97" t="s">
+        <v>11</v>
+      </c>
+      <c r="E97">
+        <v>1</v>
+      </c>
+      <c r="F97">
+        <v>64</v>
+      </c>
+      <c r="L97" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>244</v>
+      </c>
+      <c r="C98" t="s">
+        <v>244</v>
+      </c>
+      <c r="D98" t="s">
+        <v>158</v>
+      </c>
+      <c r="E98">
+        <v>1</v>
+      </c>
+      <c r="F98">
+        <v>64</v>
+      </c>
+      <c r="L98" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>245</v>
+      </c>
+      <c r="C99" t="s">
+        <v>245</v>
+      </c>
+      <c r="D99" t="s">
+        <v>11</v>
+      </c>
+      <c r="E99">
+        <v>1</v>
+      </c>
+      <c r="F99">
+        <v>64</v>
+      </c>
+      <c r="L99" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>246</v>
+      </c>
+      <c r="C100" t="s">
+        <v>246</v>
+      </c>
+      <c r="D100" t="s">
+        <v>158</v>
+      </c>
+      <c r="E100">
+        <v>1</v>
+      </c>
+      <c r="F100">
+        <v>64</v>
+      </c>
+      <c r="L100" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>247</v>
+      </c>
+      <c r="C101" t="s">
+        <v>247</v>
+      </c>
+      <c r="D101" t="s">
+        <v>11</v>
+      </c>
+      <c r="E101">
+        <v>1</v>
+      </c>
+      <c r="F101">
+        <v>64</v>
+      </c>
+      <c r="L101" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102" t="s">
+        <v>248</v>
+      </c>
+      <c r="C102" t="s">
+        <v>248</v>
+      </c>
+      <c r="D102" t="s">
+        <v>158</v>
+      </c>
+      <c r="E102">
+        <v>1</v>
+      </c>
+      <c r="F102">
+        <v>64</v>
+      </c>
+      <c r="L102" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103" t="s">
+        <v>249</v>
+      </c>
+      <c r="C103" t="s">
+        <v>249</v>
+      </c>
+      <c r="D103" t="s">
+        <v>11</v>
+      </c>
+      <c r="E103">
+        <v>1</v>
+      </c>
+      <c r="F103">
+        <v>64</v>
+      </c>
+      <c r="L103" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104" t="s">
+        <v>250</v>
+      </c>
+      <c r="C104" t="s">
+        <v>250</v>
+      </c>
+      <c r="D104" t="s">
+        <v>158</v>
+      </c>
+      <c r="E104">
+        <v>1</v>
+      </c>
+      <c r="F104">
+        <v>64</v>
+      </c>
+      <c r="L104" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105" t="s">
+        <v>251</v>
+      </c>
+      <c r="C105" t="s">
+        <v>251</v>
+      </c>
+      <c r="D105" t="s">
+        <v>11</v>
+      </c>
+      <c r="E105">
+        <v>1</v>
+      </c>
+      <c r="F105">
+        <v>64</v>
+      </c>
+      <c r="L105" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106" t="s">
+        <v>252</v>
+      </c>
+      <c r="C106" t="s">
+        <v>252</v>
+      </c>
+      <c r="D106" t="s">
+        <v>158</v>
+      </c>
+      <c r="E106">
+        <v>1</v>
+      </c>
+      <c r="F106">
+        <v>64</v>
+      </c>
+      <c r="L106" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107" t="s">
+        <v>253</v>
+      </c>
+      <c r="C107" t="s">
+        <v>253</v>
+      </c>
+      <c r="D107" t="s">
+        <v>11</v>
+      </c>
+      <c r="E107">
+        <v>1</v>
+      </c>
+      <c r="F107">
+        <v>64</v>
+      </c>
+      <c r="L107" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108" t="s">
+        <v>254</v>
+      </c>
+      <c r="C108" t="s">
+        <v>254</v>
+      </c>
+      <c r="D108" t="s">
+        <v>158</v>
+      </c>
+      <c r="E108">
+        <v>1</v>
+      </c>
+      <c r="F108">
+        <v>64</v>
+      </c>
+      <c r="L108" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>108</v>
+      </c>
+      <c r="B109" t="s">
+        <v>255</v>
+      </c>
+      <c r="C109" t="s">
+        <v>255</v>
+      </c>
+      <c r="D109" t="s">
+        <v>11</v>
+      </c>
+      <c r="E109">
+        <v>1</v>
+      </c>
+      <c r="F109">
+        <v>64</v>
+      </c>
+      <c r="L109" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>109</v>
+      </c>
+      <c r="B110" t="s">
+        <v>256</v>
+      </c>
+      <c r="C110" t="s">
+        <v>256</v>
+      </c>
+      <c r="D110" t="s">
+        <v>158</v>
+      </c>
+      <c r="E110">
+        <v>1</v>
+      </c>
+      <c r="F110">
+        <v>64</v>
+      </c>
+      <c r="L110" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>110</v>
+      </c>
+      <c r="B111" t="s">
+        <v>257</v>
+      </c>
+      <c r="C111" t="s">
+        <v>257</v>
+      </c>
+      <c r="D111" t="s">
+        <v>11</v>
+      </c>
+      <c r="E111">
+        <v>1</v>
+      </c>
+      <c r="F111">
+        <v>64</v>
+      </c>
+      <c r="L111" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>111</v>
+      </c>
+      <c r="B112" t="s">
+        <v>258</v>
+      </c>
+      <c r="C112" t="s">
+        <v>258</v>
+      </c>
+      <c r="D112" t="s">
+        <v>158</v>
+      </c>
+      <c r="E112">
+        <v>1</v>
+      </c>
+      <c r="F112">
+        <v>64</v>
+      </c>
+      <c r="L112" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113" t="s">
+        <v>259</v>
+      </c>
+      <c r="C113" t="s">
+        <v>259</v>
+      </c>
+      <c r="D113" t="s">
+        <v>11</v>
+      </c>
+      <c r="E113">
+        <v>1</v>
+      </c>
+      <c r="F113">
+        <v>64</v>
+      </c>
+      <c r="L113" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <v>113</v>
+      </c>
+      <c r="B114" t="s">
+        <v>260</v>
+      </c>
+      <c r="C114" t="s">
+        <v>260</v>
+      </c>
+      <c r="D114" t="s">
+        <v>158</v>
+      </c>
+      <c r="E114">
+        <v>1</v>
+      </c>
+      <c r="F114">
+        <v>64</v>
+      </c>
+      <c r="L114" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115" t="s">
+        <v>261</v>
+      </c>
+      <c r="C115" t="s">
+        <v>261</v>
+      </c>
+      <c r="D115" t="s">
+        <v>11</v>
+      </c>
+      <c r="E115">
+        <v>1</v>
+      </c>
+      <c r="F115">
+        <v>64</v>
+      </c>
+      <c r="L115" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116" t="s">
+        <v>262</v>
+      </c>
+      <c r="C116" t="s">
+        <v>262</v>
+      </c>
+      <c r="D116" t="s">
+        <v>158</v>
+      </c>
+      <c r="E116">
+        <v>1</v>
+      </c>
+      <c r="F116">
+        <v>64</v>
+      </c>
+      <c r="L116" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <v>116</v>
+      </c>
+      <c r="B117" t="s">
+        <v>263</v>
+      </c>
+      <c r="C117" t="s">
+        <v>263</v>
+      </c>
+      <c r="D117" t="s">
+        <v>11</v>
+      </c>
+      <c r="E117">
+        <v>1</v>
+      </c>
+      <c r="F117">
+        <v>64</v>
+      </c>
+      <c r="L117" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118" t="s">
+        <v>264</v>
+      </c>
+      <c r="C118" t="s">
+        <v>264</v>
+      </c>
+      <c r="D118" t="s">
+        <v>158</v>
+      </c>
+      <c r="E118">
+        <v>1</v>
+      </c>
+      <c r="F118">
+        <v>64</v>
+      </c>
+      <c r="L118" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="B119" t="s">
+        <v>265</v>
+      </c>
+      <c r="C119" t="s">
+        <v>265</v>
+      </c>
+      <c r="D119" t="s">
+        <v>11</v>
+      </c>
+      <c r="E119">
+        <v>1</v>
+      </c>
+      <c r="F119">
+        <v>64</v>
+      </c>
+      <c r="L119" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <v>119</v>
+      </c>
+      <c r="B120" t="s">
+        <v>266</v>
+      </c>
+      <c r="C120" t="s">
+        <v>266</v>
+      </c>
+      <c r="D120" t="s">
+        <v>158</v>
+      </c>
+      <c r="E120">
+        <v>1</v>
+      </c>
+      <c r="F120">
+        <v>64</v>
+      </c>
+      <c r="L120" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121" t="s">
+        <v>267</v>
+      </c>
+      <c r="C121" t="s">
+        <v>267</v>
+      </c>
+      <c r="D121" t="s">
+        <v>11</v>
+      </c>
+      <c r="E121">
+        <v>1</v>
+      </c>
+      <c r="F121">
+        <v>64</v>
+      </c>
+      <c r="L121" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <v>121</v>
+      </c>
+      <c r="B122" t="s">
+        <v>268</v>
+      </c>
+      <c r="C122" t="s">
+        <v>268</v>
+      </c>
+      <c r="D122" t="s">
+        <v>158</v>
+      </c>
+      <c r="E122">
+        <v>1</v>
+      </c>
+      <c r="F122">
+        <v>64</v>
+      </c>
+      <c r="L122" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <v>122</v>
+      </c>
+      <c r="B123" t="s">
+        <v>269</v>
+      </c>
+      <c r="C123" t="s">
+        <v>269</v>
+      </c>
+      <c r="D123" t="s">
+        <v>11</v>
+      </c>
+      <c r="E123">
+        <v>1</v>
+      </c>
+      <c r="F123">
+        <v>64</v>
+      </c>
+      <c r="L123" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A124">
+        <v>123</v>
+      </c>
+      <c r="B124" t="s">
+        <v>270</v>
+      </c>
+      <c r="C124" t="s">
+        <v>270</v>
+      </c>
+      <c r="D124" t="s">
+        <v>158</v>
+      </c>
+      <c r="E124">
+        <v>1</v>
+      </c>
+      <c r="F124">
+        <v>64</v>
+      </c>
+      <c r="L124" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A125">
+        <v>124</v>
+      </c>
+      <c r="B125" t="s">
+        <v>271</v>
+      </c>
+      <c r="C125" t="s">
+        <v>271</v>
+      </c>
+      <c r="D125" t="s">
+        <v>11</v>
+      </c>
+      <c r="E125">
+        <v>1</v>
+      </c>
+      <c r="F125">
+        <v>64</v>
+      </c>
+      <c r="L125" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A126">
+        <v>125</v>
+      </c>
+      <c r="B126" t="s">
+        <v>272</v>
+      </c>
+      <c r="C126" t="s">
+        <v>272</v>
+      </c>
+      <c r="D126" t="s">
+        <v>158</v>
+      </c>
+      <c r="E126">
+        <v>1</v>
+      </c>
+      <c r="F126">
+        <v>64</v>
+      </c>
+      <c r="L126" t="s">
+        <v>302</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L57">
     <sortCondition ref="A2:A57"/>

</xml_diff>